<commit_message>
adding customer notification to parent case, and attaching letter
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953923$\Bank-Account-Change-Letters\Bank Account Change Letters\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C297673E-8B05-47D7-97F8-A733AC103A60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB63F3DF-4516-4FF2-8F4E-AB61DAE8382E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t>CustomerNotificationSubject</t>
   </si>
   <si>
-    <t>Bank Account Changes Letter Sent</t>
-  </si>
-  <si>
     <t>DocumentType</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>C:\Users\x953923\Desktop\Network Directory\</t>
+  </si>
+  <si>
+    <t>Bank letters issued to all parties with full or legal permissions</t>
   </si>
 </sst>
 </file>
@@ -332,12 +332,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -352,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -377,6 +383,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +905,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>46</v>
@@ -992,42 +1004,42 @@
         <v>48</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1047,65 +1059,65 @@
         <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="C29" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="C33" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
edited config, attach letter to customer notification, add customer notification and resolve case
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB63F3DF-4516-4FF2-8F4E-AB61DAE8382E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA355E6-618D-4BE4-881A-ACB7F8972509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>timeoutS</t>
   </si>
@@ -273,19 +273,7 @@
     <t>Resolution type when resolving the case</t>
   </si>
   <si>
-    <t>ChildResolutionInput</t>
-  </si>
-  <si>
-    <t>Letter Sent</t>
-  </si>
-  <si>
-    <t>ParentResolutionInput</t>
-  </si>
-  <si>
     <t>Resolved</t>
-  </si>
-  <si>
-    <t>Resolution input when resolving the child case</t>
   </si>
   <si>
     <t>Resolution input when resolving the parent case</t>
@@ -299,6 +287,9 @@
   </si>
   <si>
     <t>Bank letters issued to all parties with full or legal permissions</t>
+  </si>
+  <si>
+    <t>ResolutionInput</t>
   </si>
 </sst>
 </file>
@@ -439,8 +430,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -747,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +896,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>46</v>
@@ -1004,7 +995,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>53</v>
@@ -1059,7 +1050,7 @@
         <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>76</v>
@@ -1100,53 +1091,42 @@
     </row>
     <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>85</v>
+      <c r="A33" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>18</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>47</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to wording on breakpoint 1 & 3, checking through all crm workflows, and removing unneeded info in the config
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA355E6-618D-4BE4-881A-ACB7F8972509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8525AA-1E82-4698-BAFB-B28D773AA504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>timeoutS</t>
   </si>
@@ -189,63 +189,15 @@
     <t>Filepath for the shared folder where the pdfs will be copied to</t>
   </si>
   <si>
-    <t>C:\Users\{0}\Desktop\Bank Account Change Letter Logs_{1}.xlsx</t>
-  </si>
-  <si>
     <t>WorkpackageName</t>
   </si>
   <si>
-    <t>Bank Account Change Letter</t>
-  </si>
-  <si>
     <t>Name of the workpackage</t>
   </si>
   <si>
-    <t>LetterAttachedTitle</t>
-  </si>
-  <si>
-    <t>Letter Attached</t>
-  </si>
-  <si>
-    <t>CaseTitle</t>
-  </si>
-  <si>
-    <t>Bank Account Changes</t>
-  </si>
-  <si>
-    <t>CaseOrigin</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>CaseType</t>
-  </si>
-  <si>
-    <t>Telephone Call</t>
-  </si>
-  <si>
-    <t>Case Title for editing child case details</t>
-  </si>
-  <si>
-    <t>Case Origin for editing child case details</t>
-  </si>
-  <si>
-    <t>Case Type for editing child case details</t>
-  </si>
-  <si>
     <t>Regex for editing child regex details</t>
   </si>
   <si>
-    <t>CorrectFormType</t>
-  </si>
-  <si>
-    <t>Information</t>
-  </si>
-  <si>
-    <t>Correct form type for the customer notification</t>
-  </si>
-  <si>
     <t>CustomerNotificationSubject</t>
   </si>
   <si>
@@ -259,9 +211,6 @@
   </si>
   <si>
     <t>Document Type for customer notification</t>
-  </si>
-  <si>
-    <t>Letter Attached Title for customer notification</t>
   </si>
   <si>
     <t>ResolutionType</t>
@@ -290,6 +239,12 @@
   </si>
   <si>
     <t>ResolutionInput</t>
+  </si>
+  <si>
+    <t>RPA Bank Change Letter</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\Bank Change Letter Logs_{1}.xlsx</t>
   </si>
 </sst>
 </file>
@@ -323,18 +278,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -349,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -374,12 +323,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -738,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +839,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>46</v>
@@ -940,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -948,13 +891,13 @@
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -995,43 +938,43 @@
         <v>48</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="10" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="C26" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,94 +982,39 @@
         <v>70</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>86</v>
+      <c r="A28" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>75</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed where config is reading from for deploying, published new package and deleted old ones
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8525AA-1E82-4698-BAFB-B28D773AA504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCBF38B-830B-4753-96EC-EC3CDB592473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,10 +241,10 @@
     <t>ResolutionInput</t>
   </si>
   <si>
-    <t>RPA Bank Change Letter</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Desktop\Bank Change Letter Logs_{1}.xlsx</t>
+    <t>RPA Bank Account Change Letter</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\Bank Account Change Letter Logs_{1}.xlsx</t>
   </si>
 </sst>
 </file>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes to check for type of form library activity and check case form type is case ui form
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCBF38B-830B-4753-96EC-EC3CDB592473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5D2CC-1855-4002-8645-4E4DB2AE3958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,7 +684,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>21</v>
@@ -729,7 +729,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -740,7 +740,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -751,7 +751,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
changes to add an attachment (paperclip) activities, add note activies, and check form type to continue on error for when not visible on some users views
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5D2CC-1855-4002-8645-4E4DB2AE3958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903302C9-CD30-4A9A-91CA-5AC859045C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>timeoutS</t>
   </si>
@@ -245,13 +245,25 @@
   </si>
   <si>
     <t>C:\Users\{0}\Desktop\Bank Account Change Letter Logs_{1}.xlsx</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/login</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/main</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +289,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -324,11 +343,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -373,12 +398,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F307B7F0-6479-4F82-9772-F27D774404D3}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +721,7 @@
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -705,15 +731,18 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -724,7 +753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -735,7 +764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -746,7 +775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -757,7 +786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -768,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -779,7 +808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -790,7 +819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -801,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -812,7 +841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -823,7 +852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -834,7 +863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -845,40 +874,49 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -889,7 +927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -900,7 +938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
@@ -911,7 +949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -922,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -933,7 +971,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -944,7 +982,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
@@ -955,7 +993,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
@@ -966,7 +1004,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>62</v>
       </c>
@@ -977,7 +1015,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -988,7 +1026,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -996,7 +1034,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -1007,7 +1045,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
added in scheme type and scheme year to edit customer notification worfklow, and updated crm library package
</commit_message>
<xml_diff>
--- a/Bank Account Change Letters/Documents/Config/config.xlsx
+++ b/Bank Account Change Letters/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Bank-Change-Letter\Bank Account Change Letters\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903302C9-CD30-4A9A-91CA-5AC859045C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315E990B-10C6-4AD0-A96B-F2EDE34DE31C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>timeoutS</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
+  </si>
+  <si>
+    <t>SchemeType</t>
+  </si>
+  <si>
+    <t>SchemeYear</t>
+  </si>
+  <si>
+    <t>Not Scheme Specific</t>
+  </si>
+  <si>
+    <t>Not Year Specific</t>
+  </si>
+  <si>
+    <t>Scheme Type for customer notification</t>
+  </si>
+  <si>
+    <t>Scheme Year for customer notification</t>
   </si>
 </sst>
 </file>
@@ -398,8 +416,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="2"/>
@@ -707,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,53 +1024,75 @@
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>